<commit_message>
updates to Material list
</commit_message>
<xml_diff>
--- a/sample_team.xlsx
+++ b/sample_team.xlsx
@@ -2,12 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PinnamaneniJa\Desktop\fmp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="210" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="210" windowWidth="21555" windowHeight="9375"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sample_team" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,106 +26,106 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Full Time %</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Run Out</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
     <t>a</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Full Time %</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Run Out</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Contract</t>
-  </si>
-  <si>
-    <t>abc</t>
+    <t>kllk</t>
+  </si>
+  <si>
+    <t>analyst 1</t>
+  </si>
+  <si>
+    <t>On</t>
   </si>
   <si>
     <t>def</t>
   </si>
   <si>
+    <t>analyst 5</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
     <t>ghi</t>
   </si>
   <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>pm 1</t>
+  </si>
+  <si>
     <t>jkl</t>
   </si>
   <si>
+    <t>jff</t>
+  </si>
+  <si>
+    <t>pm 2</t>
+  </si>
+  <si>
     <t>mno</t>
   </si>
   <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>engineer 4</t>
+  </si>
+  <si>
     <t>pqr</t>
   </si>
   <si>
+    <t>engineer 2</t>
+  </si>
+  <si>
     <t>stu</t>
   </si>
   <si>
+    <t>kds</t>
+  </si>
+  <si>
     <t>vw</t>
   </si>
   <si>
+    <t>mm 2</t>
+  </si>
+  <si>
     <t>xyz</t>
   </si>
   <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>ccc</t>
-  </si>
-  <si>
-    <t>kllk</t>
-  </si>
-  <si>
-    <t>jff</t>
-  </si>
-  <si>
-    <t>kds</t>
-  </si>
-  <si>
     <t>nmo</t>
   </si>
   <si>
-    <t>analyst 1</t>
-  </si>
-  <si>
-    <t>analyst 5</t>
-  </si>
-  <si>
-    <t>pm 1</t>
-  </si>
-  <si>
-    <t>pm 2</t>
-  </si>
-  <si>
-    <t>engineer 4</t>
-  </si>
-  <si>
-    <t>engineer 2</t>
-  </si>
-  <si>
-    <t>mm 2</t>
-  </si>
-  <si>
     <t>scientist 1</t>
   </si>
   <si>
-    <t>On</t>
-  </si>
-  <si>
-    <t>Off</t>
-  </si>
-  <si>
-    <t>Fund To (Overrides date in program)</t>
+    <t>Fund To</t>
   </si>
 </sst>
 </file>
@@ -439,84 +444,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>33</v>
+      <c r="H1">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="1">
-        <v>47120</v>
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="G3" s="1">
         <v>47120</v>
@@ -524,22 +532,22 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E4">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1">
         <v>47120</v>
@@ -547,22 +555,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>0.8</v>
+      </c>
+      <c r="F5" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
       </c>
       <c r="G5" s="1">
         <v>47120</v>
@@ -570,45 +578,45 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
       <c r="E6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G6" s="1">
-        <v>47239</v>
+        <v>47120</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1">
         <v>47239</v>
@@ -616,45 +624,45 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
       <c r="G8" s="1">
-        <v>47120</v>
+        <v>47239</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="G9" s="1">
         <v>47120</v>
@@ -662,29 +670,51 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G10" s="1">
         <v>47120</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="1">
+        <v>47120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>